<commit_message>
Products are being displayed succesfully at Main Shop in the products section
</commit_message>
<xml_diff>
--- a/Presentation/Content/Items/Prekes.xlsx
+++ b/Presentation/Content/Items/Prekes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_8AD71C61E4FF7B97CBECFC0E7F81D7E9C45A23E3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E0A4E87F-E012-4AFD-85ED-A4DF29390D5C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="170">
   <si>
     <t>Product Name</t>
   </si>
@@ -48,9 +49,6 @@
     <t xml:space="preserve">Choke </t>
   </si>
   <si>
-    <t>http://terrasport.lt/10875-thickbox_default/riedlente-choke-logo-series-pinky.jpg</t>
-  </si>
-  <si>
     <t>SK75623</t>
   </si>
   <si>
@@ -99,9 +97,6 @@
     <t>Choke Skull Series Homegrown Evo</t>
   </si>
   <si>
-    <t>http://terrasport.lt/9140-thickbox_default/riedlente-choke-skull-series-homegrown-evo.jpg</t>
-  </si>
-  <si>
     <t>SK564523</t>
   </si>
   <si>
@@ -123,9 +118,6 @@
     <t>Choke Heavy Metal Silver</t>
   </si>
   <si>
-    <t>http://terrasport.lt/10755-thickbox_default/riedlente-choke-heavy-metal-silver.jpg</t>
-  </si>
-  <si>
     <t>SK951236</t>
   </si>
   <si>
@@ -183,9 +175,6 @@
     <t>171.27</t>
   </si>
   <si>
-    <t>http://www.vejobroliai.lt/3673-thickbox_default/mindless-voodoo-lakota-dt-.jpg</t>
-  </si>
-  <si>
     <t>SK321785</t>
   </si>
   <si>
@@ -195,9 +184,6 @@
     <t>29.75“</t>
   </si>
   <si>
-    <t>http://www.vejobroliai.lt/3933-thickbox_default/fuck-the-rules.jpg</t>
-  </si>
-  <si>
     <t>SK862314</t>
   </si>
   <si>
@@ -225,9 +211,6 @@
     <t>155.86</t>
   </si>
   <si>
-    <t>http://terrasport.lt/10621-thickbox_default/longboard-as-tempish-flow-46.jpg</t>
-  </si>
-  <si>
     <t>SK452354</t>
   </si>
   <si>
@@ -255,9 +238,6 @@
     <t>158.26</t>
   </si>
   <si>
-    <t>http://terrasport.lt/9258-thickbox_default/longboard-as-volten-imperio-ii-dropthrough.jpg</t>
-  </si>
-  <si>
     <t>SK367845</t>
   </si>
   <si>
@@ -279,9 +259,6 @@
     <t>176.22</t>
   </si>
   <si>
-    <t>http://www.vejobroliai.lt/3687-thickbox_default/seba-fr1-80-grey-rieduciai.jpg</t>
-  </si>
-  <si>
     <t>SK235487</t>
   </si>
   <si>
@@ -333,9 +310,6 @@
     <t>158.40</t>
   </si>
   <si>
-    <t>http://www.vejobroliai.lt/3197-thickbox_default/seba-fr2-80-rieduciai.jpg</t>
-  </si>
-  <si>
     <t>SK987652</t>
   </si>
   <si>
@@ -390,9 +364,6 @@
     <t>Powerslide standard Man S</t>
   </si>
   <si>
-    <t>http://terrasport.lt/10742-thickbox_default/powerslide-standard-man-apsaugu-komplektas.jpg</t>
-  </si>
-  <si>
     <t>SK321256</t>
   </si>
   <si>
@@ -429,9 +400,6 @@
     <t>Autobahn Nexus</t>
   </si>
   <si>
-    <t>http://terrasport.lt/9355-thickbox_default/ratukai-riedlentei-autobahn-nexus-52x30-100a.jpg</t>
-  </si>
-  <si>
     <t>SK126756</t>
   </si>
   <si>
@@ -462,9 +430,6 @@
     <t>Powerslide DEFCON RTS</t>
   </si>
   <si>
-    <t>http://terrasport.lt/10877-thickbox_default/rieduciu-ratukai-powerslide-defcon-rts-80mm.jpg</t>
-  </si>
-  <si>
     <t>SK513548</t>
   </si>
   <si>
@@ -483,9 +448,6 @@
     <t>SEBA Luminous</t>
   </si>
   <si>
-    <t>http://terrasport.lt/10768-thickbox_default/rieduciu-ratukai-seba-luminous-violetiniai.jpg</t>
-  </si>
-  <si>
     <t>SK189456</t>
   </si>
   <si>
@@ -501,9 +463,6 @@
     <t>73.90</t>
   </si>
   <si>
-    <t>http://terrasport.lt/10535-thickbox_default/guoliukai-wicked-sus-rustproof.jpg</t>
-  </si>
-  <si>
     <t>SK956231</t>
   </si>
   <si>
@@ -568,12 +527,15 @@
   </si>
   <si>
     <t>Kokybiškos riedutininkų apsaugos</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81gqqKQVkAL._AC_SL1500_.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -716,6 +678,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -731,10 +699,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,12 +713,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1032,27 +994,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62:D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" customWidth="1"/>
-    <col min="8" max="8" width="54.85546875" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" customWidth="1"/>
+    <col min="8" max="8" width="54.88671875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1074,10 +1036,10 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1088,33 +1050,33 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="8">
         <v>49</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1126,19 +1088,19 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1150,19 +1112,19 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1174,19 +1136,19 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1198,19 +1160,19 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1222,19 +1184,19 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1246,33 +1208,33 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="8">
+        <v>59</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="6">
-        <v>59</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1284,19 +1246,19 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1308,19 +1270,19 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1332,19 +1294,19 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1356,19 +1318,19 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1380,19 +1342,19 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1404,33 +1366,33 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="8">
+        <v>59</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="6">
-        <v>59</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="G14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1442,19 +1404,19 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1466,19 +1428,19 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1490,19 +1452,19 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1514,19 +1476,19 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1538,19 +1500,19 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -1562,33 +1524,33 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="8">
+        <v>195</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C20" s="6">
-        <v>195</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="G20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="H20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -1600,19 +1562,19 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="6"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="8"/>
       <c r="H21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1624,19 +1586,19 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="6"/>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="8"/>
       <c r="H22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -1648,19 +1610,19 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="6"/>
+    <row r="23" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1672,19 +1634,19 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="6"/>
+    <row r="24" spans="1:18" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="8"/>
       <c r="H24" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1696,31 +1658,31 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1732,19 +1694,19 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="6"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="8"/>
       <c r="H26" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1756,19 +1718,19 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="6"/>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="8"/>
       <c r="H27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1780,19 +1742,19 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="6"/>
+    <row r="28" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="8"/>
       <c r="H28" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1804,33 +1766,33 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C29" s="6">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="8">
         <v>139</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>45</v>
+      <c r="D29" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -1842,19 +1804,19 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
       <c r="H30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1866,19 +1828,19 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
       <c r="H31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1890,19 +1852,19 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
       <c r="H32" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -1914,19 +1876,19 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
       <c r="H33" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -1938,33 +1900,33 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>45</v>
+    <row r="34" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -1976,19 +1938,19 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
       <c r="H35" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2000,19 +1962,19 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
       <c r="H36" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -2024,19 +1986,19 @@
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
       <c r="H37" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -2048,19 +2010,19 @@
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
       <c r="H38" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -2072,33 +2034,33 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>45</v>
+    <row r="39" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2110,19 +2072,19 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
       <c r="H40" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -2134,19 +2096,19 @@
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
       <c r="H41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -2158,19 +2120,19 @@
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
       <c r="H42" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -2182,19 +2144,19 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
       <c r="H43" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -2206,33 +2168,33 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>89</v>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -2244,19 +2206,19 @@
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
       <c r="H45" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -2268,19 +2230,19 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
       <c r="H46" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -2292,19 +2254,19 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
       <c r="H47" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -2316,33 +2278,33 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C48" s="6">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="8">
         <v>299</v>
       </c>
-      <c r="D48" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G48" s="6" t="s">
+      <c r="D48" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="F48" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="H48" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -2354,19 +2316,19 @@
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
       <c r="H49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -2378,19 +2340,19 @@
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
       <c r="H50" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -2402,19 +2364,19 @@
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
       <c r="H51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -2426,33 +2388,33 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>89</v>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -2464,19 +2426,19 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+    <row r="53" spans="1:18" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
       <c r="H53" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -2488,33 +2450,33 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>113</v>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -2526,19 +2488,19 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="6"/>
+    <row r="55" spans="1:18" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="8"/>
       <c r="H55" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -2550,33 +2512,33 @@
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D56" s="10" t="s">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F56" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>113</v>
+      <c r="D56" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -2588,19 +2550,19 @@
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="6"/>
+    <row r="57" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="8"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="8"/>
       <c r="H57" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -2612,33 +2574,33 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C58" s="6">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A58" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" s="8">
         <v>29</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>113</v>
+      <c r="D58" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -2650,19 +2612,19 @@
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
+    <row r="59" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="8"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
       <c r="H59" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -2674,33 +2636,33 @@
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C60" s="6">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="8">
         <v>29</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>113</v>
+      <c r="D60" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -2712,19 +2674,19 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
+    <row r="61" spans="1:18" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="8"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
       <c r="H61" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -2736,33 +2698,33 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C62" s="6">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A62" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" s="8">
         <v>39</v>
       </c>
-      <c r="D62" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>113</v>
+      <c r="D62" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -2774,19 +2736,19 @@
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
+    <row r="63" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
       <c r="H63" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -2798,33 +2760,33 @@
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B64" s="7" t="s">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A64" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" s="8">
+        <v>29</v>
+      </c>
+      <c r="D64" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C64" s="6">
-        <v>29</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>17</v>
+      <c r="E64" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -2836,19 +2798,19 @@
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A65" s="8"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
       <c r="H65" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -2860,19 +2822,19 @@
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6"/>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A66" s="8"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
       <c r="H66" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -2884,19 +2846,19 @@
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
+    <row r="67" spans="1:18" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="8"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
       <c r="H67" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -2908,33 +2870,33 @@
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C68" s="6">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A68" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="8">
         <v>32</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>17</v>
+      <c r="D68" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -2946,19 +2908,19 @@
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A69" s="8"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
       <c r="H69" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -2970,19 +2932,19 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
+    <row r="70" spans="1:18" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
       <c r="H70" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -2994,33 +2956,33 @@
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B71" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C71" s="6">
+      <c r="C71" s="8">
         <v>30</v>
       </c>
-      <c r="D71" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>17</v>
+      <c r="D71" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -3032,19 +2994,19 @@
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A72" s="8"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
       <c r="H72" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
@@ -3056,19 +3018,19 @@
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
+    <row r="73" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="8"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
       <c r="H73" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
@@ -3080,27 +3042,27 @@
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
     </row>
-    <row r="74" spans="1:18" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="4"/>
@@ -3114,7 +3076,7 @@
       <c r="Q74" s="2"/>
       <c r="R74" s="2"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3134,7 +3096,7 @@
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3154,7 +3116,7 @@
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3174,7 +3136,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3194,7 +3156,7 @@
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3214,7 +3176,7 @@
       <c r="Q79" s="2"/>
       <c r="R79" s="2"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3234,7 +3196,7 @@
       <c r="Q80" s="2"/>
       <c r="R80" s="2"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -3254,7 +3216,7 @@
       <c r="Q81" s="2"/>
       <c r="R81" s="2"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3274,7 +3236,7 @@
       <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3294,7 +3256,7 @@
       <c r="Q83" s="2"/>
       <c r="R83" s="2"/>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3314,7 +3276,7 @@
       <c r="Q84" s="2"/>
       <c r="R84" s="2"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3334,7 +3296,7 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3354,7 +3316,7 @@
       <c r="Q86" s="2"/>
       <c r="R86" s="2"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3374,7 +3336,7 @@
       <c r="Q87" s="2"/>
       <c r="R87" s="2"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3394,7 +3356,7 @@
       <c r="Q88" s="2"/>
       <c r="R88" s="2"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3414,7 +3376,7 @@
       <c r="Q89" s="2"/>
       <c r="R89" s="2"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3434,7 +3396,7 @@
       <c r="Q90" s="2"/>
       <c r="R90" s="2"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3454,7 +3416,7 @@
       <c r="Q91" s="2"/>
       <c r="R91" s="2"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3474,7 +3436,7 @@
       <c r="Q92" s="2"/>
       <c r="R92" s="2"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3494,7 +3456,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3514,7 +3476,7 @@
       <c r="Q94" s="2"/>
       <c r="R94" s="2"/>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3534,7 +3496,7 @@
       <c r="Q95" s="2"/>
       <c r="R95" s="2"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3554,7 +3516,7 @@
       <c r="Q96" s="2"/>
       <c r="R96" s="2"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3574,7 +3536,7 @@
       <c r="Q97" s="2"/>
       <c r="R97" s="2"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3594,7 +3556,7 @@
       <c r="Q98" s="2"/>
       <c r="R98" s="2"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3614,7 +3576,7 @@
       <c r="Q99" s="2"/>
       <c r="R99" s="2"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3634,7 +3596,7 @@
       <c r="Q100" s="2"/>
       <c r="R100" s="2"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3654,7 +3616,7 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3674,7 +3636,7 @@
       <c r="Q102" s="2"/>
       <c r="R102" s="2"/>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3694,7 +3656,7 @@
       <c r="Q103" s="2"/>
       <c r="R103" s="2"/>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3714,7 +3676,7 @@
       <c r="Q104" s="2"/>
       <c r="R104" s="2"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3734,7 +3696,7 @@
       <c r="Q105" s="2"/>
       <c r="R105" s="2"/>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3754,7 +3716,7 @@
       <c r="Q106" s="2"/>
       <c r="R106" s="2"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3774,7 +3736,7 @@
       <c r="Q107" s="2"/>
       <c r="R107" s="2"/>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3794,7 +3756,7 @@
       <c r="Q108" s="2"/>
       <c r="R108" s="2"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3814,7 +3776,7 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3834,7 +3796,7 @@
       <c r="Q110" s="2"/>
       <c r="R110" s="2"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3854,7 +3816,7 @@
       <c r="Q111" s="2"/>
       <c r="R111" s="2"/>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3874,7 +3836,7 @@
       <c r="Q112" s="2"/>
       <c r="R112" s="2"/>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3894,7 +3856,7 @@
       <c r="Q113" s="2"/>
       <c r="R113" s="2"/>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3916,28 +3878,104 @@
     </row>
   </sheetData>
   <mergeCells count="134">
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="E2:E7"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="F14:F19"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="G64:G67"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="G39:G43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="F44:F47"/>
+    <mergeCell ref="G44:G47"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="E39:E43"/>
+    <mergeCell ref="F39:F43"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="G34:G38"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="F29:F33"/>
     <mergeCell ref="G20:G24"/>
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B25:B28"/>
@@ -3952,126 +3990,49 @@
     <mergeCell ref="D20:D24"/>
     <mergeCell ref="E20:E24"/>
     <mergeCell ref="F20:F24"/>
-    <mergeCell ref="G29:G33"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="D34:D38"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="G34:G38"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="F29:F33"/>
-    <mergeCell ref="G39:G43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="F44:F47"/>
-    <mergeCell ref="G44:G47"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="E39:E43"/>
-    <mergeCell ref="F39:F43"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G68:G70"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="F14:F19"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="G8:G13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2"/>
-    <hyperlink ref="D14" r:id="rId3"/>
-    <hyperlink ref="D20" r:id="rId4"/>
-    <hyperlink ref="D25" r:id="rId5"/>
-    <hyperlink ref="D29" r:id="rId6"/>
-    <hyperlink ref="D34" r:id="rId7"/>
-    <hyperlink ref="D39" r:id="rId8"/>
-    <hyperlink ref="D44" r:id="rId9"/>
-    <hyperlink ref="D48" r:id="rId10"/>
-    <hyperlink ref="D52" r:id="rId11"/>
-    <hyperlink ref="D54" r:id="rId12"/>
-    <hyperlink ref="D56" r:id="rId13"/>
-    <hyperlink ref="D58" r:id="rId14"/>
-    <hyperlink ref="D60" r:id="rId15"/>
-    <hyperlink ref="D62" r:id="rId16"/>
-    <hyperlink ref="D64" r:id="rId17"/>
-    <hyperlink ref="D68" r:id="rId18"/>
-    <hyperlink ref="D71" r:id="rId19"/>
-    <hyperlink ref="D74" r:id="rId20"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D25" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D29" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D44" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D52" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D54" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D56" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D58" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D60" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D62" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D64" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D68" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D71" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D8" r:id="rId16" xr:uid="{B82EB1ED-CD70-4227-B2FD-0F41DC9BFDFB}"/>
+    <hyperlink ref="D14" r:id="rId17" xr:uid="{653B9A32-E7F9-4084-B822-3112C0BBA48E}"/>
+    <hyperlink ref="D34" r:id="rId18" xr:uid="{3A3D877E-DF9A-42F4-8896-612695F978B4}"/>
+    <hyperlink ref="D39" r:id="rId19" xr:uid="{E1B05153-8CED-4912-9169-13E4520AE7D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>